<commit_message>
Orden de archivos y documentos
</commit_message>
<xml_diff>
--- a/Homologacion Topicos.xlsx
+++ b/Homologacion Topicos.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\juako\Desktop\X\MEMORIA\Desarrollo\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\juako\Desktop\X\MEMORIA\Memoria\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8327DD1-618E-49BF-815D-1E375311878F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{420A889A-3EF6-45EB-8931-CD59B56EB49F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-135" windowWidth="29040" windowHeight="15720" xr2:uid="{DDE7E594-D44D-4722-974B-23C002C22030}"/>
   </bookViews>
   <sheets>
     <sheet name="Homologación" sheetId="1" r:id="rId1"/>
+    <sheet name="Hoja1" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="341" uniqueCount="181">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="410" uniqueCount="245">
   <si>
     <t>Topico</t>
   </si>
@@ -605,6 +606,198 @@
   </si>
   <si>
     <t>Columna3</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Disposiciones constitucionales no sujetas a reforma</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Procedimiento de reforma constitucional</t>
+  </si>
+  <si>
+    <t>Cultura e Identidad</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Grupos Indígenas</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Idioma</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Nacionalidad</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Raza y Etnicidad</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Religión</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Normas y Procedimientos Electorales</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Partidos Políticos</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Referendos e Iniciativas</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Sufragio y Participación Electoral</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Supervisión Electoral</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Estructura del Ejecutivo</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Fuerzas Armadas</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Gabinete</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Independencia y Facultades del Ejecutivo</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Jefe de Estado</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Jefe de Gobierno</t>
+  </si>
+  <si>
+    <t>Federalismo</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Estructura del Estado</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Facultad Legislativa</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Secesión y Anexión</t>
+  </si>
+  <si>
+    <t>Normas Internacionales</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Política Exterior</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Referencias Explícitas al Derecho Internacional</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Tratados</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Autonomía y Facultades del Judicial</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Corte Suprema</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Estructura del Poder Judicial</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Revisión Judicial</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Tribunal Constitucional</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Tribunal Electoral</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Tribunales administrativos</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Tribunales ordinarios</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Destitución y Sustitución</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Estructura de las cámaras legislativas</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Independencia y Facultades del Legislativo</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Legislación</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Legislación Especial</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Primera Cámara</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Reglas y Restricciones Legislativas</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Segunda Cámara</t>
+  </si>
+  <si>
+    <t>Principios y Símbolos</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Definición del Estado y Símbolos</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Principios Básicos</t>
+  </si>
+  <si>
+    <t>Regulación y Supervisión</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Elecciones</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Medios de comunicación</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Social Issues</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Órganos Autónomos y Comisiones</t>
+  </si>
+  <si>
+    <t>Derechos y Deberes</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Deberes Ciudadanos</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Deberes Generales</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Derechos Civiles y Políticos</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Derechos Económicos</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Derechos Procesales</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Derechos Sociales</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Derechos a la Integridad Física</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Derechos de Igualdad, Género y Minoría</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Ejecución</t>
+  </si>
+  <si>
+    <t>Secciones Especiales</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Disposiciones transitorias</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Preámbulo</t>
   </si>
 </sst>
 </file>
@@ -1087,7 +1280,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="94">
+  <cellXfs count="90">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1282,26 +1475,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1317,7 +1498,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1842,8 +2023,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1514D99F-C164-40CA-B445-AEE50942FCF5}">
   <dimension ref="A1:H56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E58" sqref="E58"/>
+    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="E59" sqref="E59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2732,7 +2913,7 @@
       <c r="G39" s="68" t="s">
         <v>174</v>
       </c>
-      <c r="H39" s="80" t="s">
+      <c r="H39" s="77" t="s">
         <v>172</v>
       </c>
     </row>
@@ -2756,7 +2937,7 @@
       <c r="G40" s="67" t="s">
         <v>175</v>
       </c>
-      <c r="H40" s="81" t="s">
+      <c r="H40" s="80" t="s">
         <v>172</v>
       </c>
     </row>
@@ -2770,7 +2951,7 @@
       <c r="E41" s="73"/>
       <c r="F41" s="59"/>
       <c r="G41" s="62"/>
-      <c r="H41" s="82"/>
+      <c r="H41" s="81"/>
     </row>
     <row r="42" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A42" s="23"/>
@@ -2782,7 +2963,7 @@
       <c r="E42" s="55"/>
       <c r="F42" s="60"/>
       <c r="G42" s="68"/>
-      <c r="H42" s="83"/>
+      <c r="H42" s="82"/>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" s="23"/>
@@ -2804,7 +2985,7 @@
       <c r="G43" s="67" t="s">
         <v>175</v>
       </c>
-      <c r="H43" s="84" t="s">
+      <c r="H43" s="75" t="s">
         <v>172</v>
       </c>
     </row>
@@ -2826,7 +3007,7 @@
       <c r="G44" s="62" t="s">
         <v>175</v>
       </c>
-      <c r="H44" s="85" t="s">
+      <c r="H44" s="76" t="s">
         <v>172</v>
       </c>
     </row>
@@ -2848,7 +3029,7 @@
       <c r="G45" s="62" t="s">
         <v>175</v>
       </c>
-      <c r="H45" s="82" t="s">
+      <c r="H45" s="81" t="s">
         <v>172</v>
       </c>
     </row>
@@ -2870,7 +3051,7 @@
       <c r="G46" s="62" t="s">
         <v>174</v>
       </c>
-      <c r="H46" s="85" t="s">
+      <c r="H46" s="76" t="s">
         <v>172</v>
       </c>
     </row>
@@ -2892,7 +3073,7 @@
       <c r="G47" s="68" t="s">
         <v>174</v>
       </c>
-      <c r="H47" s="80" t="s">
+      <c r="H47" s="77" t="s">
         <v>172</v>
       </c>
     </row>
@@ -2916,7 +3097,7 @@
       <c r="G48" s="67" t="s">
         <v>175</v>
       </c>
-      <c r="H48" s="84" t="s">
+      <c r="H48" s="75" t="s">
         <v>172</v>
       </c>
     </row>
@@ -2938,7 +3119,7 @@
       <c r="G49" s="62" t="s">
         <v>175</v>
       </c>
-      <c r="H49" s="85" t="s">
+      <c r="H49" s="76" t="s">
         <v>172</v>
       </c>
     </row>
@@ -2960,7 +3141,7 @@
       <c r="G50" s="68" t="s">
         <v>174</v>
       </c>
-      <c r="H50" s="80" t="s">
+      <c r="H50" s="77" t="s">
         <v>172</v>
       </c>
     </row>
@@ -2984,7 +3165,7 @@
       <c r="G51" s="71" t="s">
         <v>175</v>
       </c>
-      <c r="H51" s="86" t="s">
+      <c r="H51" s="78" t="s">
         <v>172</v>
       </c>
     </row>
@@ -3006,7 +3187,7 @@
       <c r="G52" s="68" t="s">
         <v>175</v>
       </c>
-      <c r="H52" s="80" t="s">
+      <c r="H52" s="77" t="s">
         <v>172</v>
       </c>
     </row>
@@ -3030,7 +3211,7 @@
       <c r="G53" s="67" t="s">
         <v>174</v>
       </c>
-      <c r="H53" s="84" t="s">
+      <c r="H53" s="75" t="s">
         <v>172</v>
       </c>
     </row>
@@ -3052,7 +3233,7 @@
       <c r="G54" s="62" t="s">
         <v>174</v>
       </c>
-      <c r="H54" s="85" t="s">
+      <c r="H54" s="76" t="s">
         <v>172</v>
       </c>
     </row>
@@ -3074,29 +3255,29 @@
       <c r="G55" s="62" t="s">
         <v>174</v>
       </c>
-      <c r="H55" s="85" t="s">
+      <c r="H55" s="76" t="s">
         <v>172</v>
       </c>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A56" s="23"/>
-      <c r="B56" s="87"/>
-      <c r="C56" s="88" t="s">
+      <c r="B56" s="83"/>
+      <c r="C56" s="84" t="s">
         <v>64</v>
       </c>
-      <c r="D56" s="89" t="s">
+      <c r="D56" s="85" t="s">
         <v>131</v>
       </c>
-      <c r="E56" s="90" t="s">
+      <c r="E56" s="86" t="s">
         <v>132</v>
       </c>
-      <c r="F56" s="91" t="s">
-        <v>170</v>
-      </c>
-      <c r="G56" s="92" t="s">
+      <c r="F56" s="87" t="s">
+        <v>170</v>
+      </c>
+      <c r="G56" s="88" t="s">
         <v>174</v>
       </c>
-      <c r="H56" s="93" t="s">
+      <c r="H56" s="89" t="s">
         <v>172</v>
       </c>
     </row>
@@ -3107,4 +3288,344 @@
     <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5863E29A-C6FA-43B0-9F95-1D0D5D322072}">
+  <dimension ref="A1:B57"/>
+  <sheetViews>
+    <sheetView topLeftCell="A23" workbookViewId="0">
+      <selection sqref="A1:B57"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="47.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>160</v>
+      </c>
+      <c r="B1" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>183</v>
+      </c>
+      <c r="B3" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>162</v>
+      </c>
+      <c r="B8" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>32</v>
+      </c>
+      <c r="B13" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>200</v>
+      </c>
+      <c r="B19" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>204</v>
+      </c>
+      <c r="B22" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B23" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B24" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>33</v>
+      </c>
+      <c r="B25" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B26" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B27" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B28" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B29" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B30" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B31" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B32" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>34</v>
+      </c>
+      <c r="B33" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B34" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B35" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B36" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B37" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B38" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B39" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B40" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>224</v>
+      </c>
+      <c r="B41" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B42" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>227</v>
+      </c>
+      <c r="B43" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B44" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B45" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B46" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>232</v>
+      </c>
+      <c r="B47" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B48" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B49" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B50" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B51" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B52" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B53" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B54" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B55" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>242</v>
+      </c>
+      <c r="B56" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B57" t="s">
+        <v>244</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>